<commit_message>
Oops, I forgot a card
</commit_message>
<xml_diff>
--- a/album2.xlsx
+++ b/album2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\o\git-repos\mtg-card-price-updater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D690EAB4-2D75-4C1F-A96E-BA76962E82A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429CCFC2-6772-45F8-86E7-92C1BA3266F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Restless Fortress</t>
+  </si>
+  <si>
+    <t>Scion of Draco</t>
+  </si>
+  <si>
+    <t>Modern Horizons 2</t>
   </si>
 </sst>
 </file>
@@ -100,7 +106,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-;_-@_-"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -133,7 +139,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,10 +587,24 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D13" s="1">
-        <f>SUM(D2:D11)</f>
-        <v>19.150000000000002</v>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="1">
+        <f>SUM(D2:D12)</f>
+        <v>21.14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>